<commit_message>
Better accuracy benchmark and printouts
</commit_message>
<xml_diff>
--- a/main/accuracy_benchmark.xlsx
+++ b/main/accuracy_benchmark.xlsx
@@ -5,43 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raulgallodagir/Code/PhilipPfeffer/picme/main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipmateopfeffer/Desktop/Stanford/Y3Q1/cs221/finalproject/picme/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D35170C0-ED22-F04D-9205-30555EF80854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACAFCCA-731F-7546-9983-66B8A2457159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{D2ADA464-C0DE-4B48-99AD-637452786337}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{D2ADA464-C0DE-4B48-99AD-637452786337}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$2:$D$13</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$2:$D$13</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>benchmark</t>
   </si>
@@ -67,6 +40,45 @@
   </si>
   <si>
     <t>new accuracy</t>
+  </si>
+  <si>
+    <t>between2and6UTC</t>
+  </si>
+  <si>
+    <t>between6and10UTC</t>
+  </si>
+  <si>
+    <t>between10and14UTC</t>
+  </si>
+  <si>
+    <t>between14and18UTC</t>
+  </si>
+  <si>
+    <t>between18and22UTC</t>
+  </si>
+  <si>
+    <t>between22and2UTC</t>
+  </si>
+  <si>
+    <t>captionContainsFood</t>
+  </si>
+  <si>
+    <t>captionContainsFollow</t>
+  </si>
+  <si>
+    <t>captionContainsAd</t>
+  </si>
+  <si>
+    <t>numFaces</t>
+  </si>
+  <si>
+    <t>face%ImageArea</t>
+  </si>
+  <si>
+    <t>previous benchmark</t>
+  </si>
+  <si>
+    <t>random choice baseline</t>
   </si>
 </sst>
 </file>
@@ -124,7 +136,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -156,11 +168,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Accuracy</a:t>
+              <a:t>Percentage Accuracy</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> without feature by index </a:t>
+              <a:t> without each Feature, Compared to Benchmark with all Features</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -226,47 +238,85 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>between2and6UTC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>between6and10UTC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>between10and14UTC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>between14and18UTC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>between18and22UTC</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>between22and2UTC</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>captionContainsFood</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>captionContainsFollow</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>captionContainsAd</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>numFaces</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>face%ImageArea</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.64912000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70175438596491202</c:v>
+                  <c:v>0.75438000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.77193000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73684210526315697</c:v>
+                  <c:v>0.71928999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82456140350877105</c:v>
+                  <c:v>0.66666999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70175438596491202</c:v>
+                  <c:v>0.68420999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73684210526315697</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75438596491228005</c:v>
+                  <c:v>0.73684000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.80701754385964897</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.59649122807017496</c:v>
+                  <c:v>0.68420999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,45 +359,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.71929824561403499</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.71929824561403499</c:v>
+                  <c:v>0.70174999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -356,6 +403,70 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-8DF2-9845-8D07-3821BCA079B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-E7E7-134B-B0D0-FAEB7C341B77}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -379,6 +490,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -426,7 +538,7 @@
         <c:axId val="1073897648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.55000000000000004"/>
+          <c:min val="0.45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -487,12 +599,95 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> without each Feature, Compared to Benchmark with all Features</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -506,7 +701,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -521,7 +716,840 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>new accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>between6and10UTC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>between10and14UTC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>between14and18UTC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>numFaces</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$26:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.80700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71929799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4151-0C47-92B7-87C3127B97BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1073928784"/>
+        <c:axId val="1073897648"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$26:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4151-0C47-92B7-87C3127B97BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$26:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4151-0C47-92B7-87C3127B97BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4151-0C47-92B7-87C3127B97BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1073928784"/>
+        <c:axId val="1073897648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1073928784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1073897648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1073897648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1073928784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentage Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> without each Feature, Compared to Benchmark with all Features</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>new accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>between6and10UTC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>between10and14UTC</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>between14and18UTC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>numFaces</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$43:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.82455999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82455999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2584-224D-8D93-CBB708B129E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1073928784"/>
+        <c:axId val="1073897648"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78947000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2584-224D-8D93-CBB708B129E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$43:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70174999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2584-224D-8D93-CBB708B129E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2584-224D-8D93-CBB708B129E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$43:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.82455999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82455999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2584-224D-8D93-CBB708B129E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1073928784"/>
+        <c:axId val="1073897648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1073928784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1073897648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1073897648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1073928784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -606,7 +1634,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1114,15 +3228,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>485140</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>751840</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>200660</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1142,6 +3256,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>538480</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>805180</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBD7125A-9283-1541-B699-08A47FD59BA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>58420</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480785F9-E6CD-B249-9E7B-71D034AADBB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1447,20 +3637,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2866E2-B1B2-644F-8F3A-E5A23E085AF9}">
-  <dimension ref="C1:E13"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1469,136 +3664,294 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.64912000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.75438000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.77193000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.71928999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.70174999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.66666999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.68420999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.70174999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.70174999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E11">
+        <v>0.73684000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.68420999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E2">
-        <v>0.71929824561403499</v>
+      <c r="E25" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D26">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.71929799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D28">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0.78947000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="C29">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D29">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E3">
-        <v>0.70175438596491202</v>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E4">
-        <v>0.71929824561403499</v>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>0.5</v>
+      </c>
+      <c r="C43">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D43">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E43">
+        <v>0.82455999999999996</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E5">
-        <v>0.73684210526315697</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E6">
-        <v>0.71929824561403499</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E7">
-        <v>0.82456140350877105</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C8">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E8">
-        <v>0.70175438596491202</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E9">
-        <v>0.73684210526315697</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E10">
-        <v>0.71929824561403499</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E11">
-        <v>0.75438596491228005</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E12">
-        <v>0.80701754385964897</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>0.71929824561403499</v>
-      </c>
-      <c r="E13">
-        <v>0.59649122807017496</v>
+      <c r="B44">
+        <v>0.5</v>
+      </c>
+      <c r="C44">
+        <v>0.70174999999999998</v>
+      </c>
+      <c r="D44">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="E44">
+        <v>0.82455999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>